<commit_message>
Implemented referential integrity checks for product static data
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/admin/static_data/tests_integration/input_data/static_data_flows.products/products.products.static-data.admin.a6i.xlsx
+++ b/src/apodeixi/controllers/admin/static_data/tests_integration/input_data/static_data_flows.products/products.products.static-data.admin.a6i.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\admin\static_data\tests_integration\input_data\static_data_flows.products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F69DEA-FC18-4A3A-85FD-765B03B0DAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E3A428-6322-48E2-AE0C-D544E8D944E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>static-data.admin.a6i.io/v1a</t>
   </si>
   <si>
-    <t>My Corporation</t>
-  </si>
-  <si>
     <t>Testing Area</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>D2:G10</t>
+  </si>
+  <si>
+    <t>My Corp</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
   <dimension ref="B1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -637,7 +637,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -653,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -661,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
@@ -669,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
@@ -677,7 +677,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -709,7 +709,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
@@ -717,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
@@ -725,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -733,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -741,7 +741,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -749,11 +749,11 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -777,48 +777,48 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
@@ -826,24 +826,24 @@
       <c r="C4" s="4"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -852,29 +852,29 @@
       <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
@@ -887,10 +887,10 @@
     </row>
     <row r="9" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -898,11 +898,11 @@
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>